<commit_message>
Refactor code to convert multiple tables
</commit_message>
<xml_diff>
--- a/Test.xlsx
+++ b/Test.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\_MyDotNetApplications\ExcelToSqlServerConvertor\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{854463AF-B6D8-4516-AC17-162830934EFA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A01EFC4-50EA-4C48-A7F5-BDADFBFEB587}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{0DD5A266-1103-4D41-85AC-E4566B2BD59C}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{0DD5A266-1103-4D41-85AC-E4566B2BD59C}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="dbo.Test" sheetId="1" r:id="rId1"/>
+    <sheet name="dbo.Test2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="17">
   <si>
     <t>TestID</t>
   </si>
@@ -66,6 +67,24 @@
   </si>
   <si>
     <t>TestContent5</t>
+  </si>
+  <si>
+    <t>Test2ID</t>
+  </si>
+  <si>
+    <t>Test2Content1</t>
+  </si>
+  <si>
+    <t>Test2Content2</t>
+  </si>
+  <si>
+    <t>Test2Content3</t>
+  </si>
+  <si>
+    <t>Test2Content4</t>
+  </si>
+  <si>
+    <t>Test2Content5</t>
   </si>
 </sst>
 </file>
@@ -421,8 +440,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{83FAF49C-DC04-44A5-B89D-A7E80BF8C6E4}">
   <dimension ref="A1:F5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F5" sqref="A1:F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -536,4 +555,123 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D38ED6DE-065A-4C8F-8CB2-977F9EE60151}">
+  <dimension ref="A1:F5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="7.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="6" width="14" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2">
+        <v>1234</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F2" s="2">
+        <v>44180</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3">
+        <v>45678</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F3" s="2">
+        <v>44181</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>5</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4">
+        <v>7890</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F4" s="2">
+        <v>44182</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>9</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5">
+        <v>1234</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F5" s="2">
+        <v>44183</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>